<commit_message>
rill-analysis: Control page display.
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/luopan.xlsx
+++ b/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/luopan.xlsx
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -204,10 +204,6 @@
   </si>
   <si>
     <t>管辖岗位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>multiselect</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -778,11 +774,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="74178560"/>
-        <c:axId val="74180096"/>
+        <c:axId val="62283136"/>
+        <c:axId val="71238784"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="74178560"/>
+        <c:axId val="62283136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -791,13 +787,13 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74180096"/>
+        <c:crossAx val="71238784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="74180096"/>
+        <c:axId val="71238784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -806,7 +802,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74178560"/>
+        <c:crossAx val="62283136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -823,7 +819,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1193,9 +1189,7 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -1214,10 +1208,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3" t="s">
@@ -1250,19 +1244,19 @@
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
+      <c r="D3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="3" t="str">
-        <f>$D1&amp;" "&amp;$D2</f>
-        <v>选择日期 用户</v>
+        <f>$D2</f>
+        <v>用户</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1273,40 +1267,40 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G4" s="3" t="str">
-        <f>$D1&amp;" "&amp;$D2&amp;" "&amp;$D3</f>
-        <v>选择日期 用户 商业产品线</v>
+        <f>$D2</f>
+        <v>用户</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7" t="s">
-        <v>14</v>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="G5" s="3" t="str">
-        <f>$D1&amp;" "&amp;$D2</f>
-        <v>选择日期 用户</v>
+        <f>$D2&amp;" "&amp;$D4</f>
+        <v>用户 商业产品线</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1338,28 +1332,28 @@
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1">
       <c r="A2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="18" customHeight="1" thickBot="1">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="14.25" thickBot="1">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="8">
         <v>40630</v>
@@ -1406,7 +1400,7 @@
     </row>
     <row r="5" spans="1:15" ht="14.25" thickBot="1">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="5">
         <v>3344110</v>
@@ -1453,7 +1447,7 @@
     </row>
     <row r="6" spans="1:15" ht="14.25" thickBot="1">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="5">
         <v>4422312</v>
@@ -1500,7 +1494,7 @@
     </row>
     <row r="7" spans="1:15" ht="14.25" thickBot="1">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="5">
         <v>2422312</v>

</xml_diff>

<commit_message>
rill-analysis: Refactor chart/pivottable/table refresh structure.
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/luopan.xlsx
+++ b/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/luopan.xlsx
@@ -4,22 +4,17 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="trend" sheetId="5" r:id="rId1"/>
-    <sheet name="table" sheetId="7" r:id="rId2"/>
-    <sheet name="_settings" sheetId="2" r:id="rId3"/>
-    <sheet name="_input" sheetId="1" r:id="rId4"/>
-    <sheet name="_input2" sheetId="8" r:id="rId5"/>
+    <sheet name="_settings" sheetId="2" r:id="rId2"/>
+    <sheet name="_input" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="trendChartDataSource" localSheetId="3">OFFSET(_input!$A4,0,0,COUNTA(_input!$A:$A)-3, COUNTA(_input!$4:$4))</definedName>
+    <definedName name="trendChartDataSource" localSheetId="2">OFFSET(_input!$A4,0,0,COUNTA(_input!$A:$A)-3, COUNTA(_input!$4:$4))</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId6"/>
-  </pivotCaches>
 </workbook>
 </file>
 
@@ -154,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -254,81 +249,13 @@
   <si>
     <t>高级经理</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>高级经理</t>
-  </si>
-  <si>
-    <t>经理A</t>
-  </si>
-  <si>
-    <t>经理A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>经理B</t>
-  </si>
-  <si>
-    <t>经理B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>经理C</t>
-  </si>
-  <si>
-    <t>经理C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>总计</t>
-  </si>
-  <si>
-    <t>岗位1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>岗位2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数据类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>日数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>点击消费项</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>环比项</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>同比项</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>新客户数项</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>点击消费</t>
-  </si>
-  <si>
-    <t>环比</t>
-  </si>
-  <si>
-    <t>新客户数</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,15 +312,6 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -479,7 +397,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -510,25 +428,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -673,11 +573,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77089792"/>
-        <c:axId val="81580800"/>
+        <c:axId val="64077184"/>
+        <c:axId val="80540032"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="77089792"/>
+        <c:axId val="64077184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -686,13 +586,13 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81580800"/>
+        <c:crossAx val="80540032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="81580800"/>
+        <c:axId val="80540032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -701,7 +601,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77089792"/>
+        <c:crossAx val="64077184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -719,7 +619,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -758,136 +658,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="作者" refreshedDate="41139.908660300927" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="3">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A5:F8" sheet="_input2"/>
-  </cacheSource>
-  <cacheFields count="6">
-    <cacheField name="岗位1" numFmtId="0">
-      <sharedItems count="1">
-        <s v="高级经理"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="岗位2" numFmtId="0">
-      <sharedItems count="3">
-        <s v="经理A"/>
-        <s v="经理B"/>
-        <s v="经理C"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="点击消费项" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="234" maxValue="543"/>
-    </cacheField>
-    <cacheField name="环比项" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="13" maxValue="41"/>
-    </cacheField>
-    <cacheField name="同比项" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="7" maxValue="23"/>
-    </cacheField>
-    <cacheField name="新客户数项" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="34" maxValue="321"/>
-    </cacheField>
-  </cacheFields>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="3">
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="345"/>
-    <n v="13"/>
-    <n v="7"/>
-    <n v="34"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <n v="234"/>
-    <n v="23"/>
-    <n v="12"/>
-    <n v="321"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <n v="543"/>
-    <n v="41"/>
-    <n v="23"/>
-    <n v="321"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pivot1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A4:D9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="6">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="2">
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="0"/>
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-  </colItems>
-  <dataFields count="3">
-    <dataField name="点击消费" fld="2" baseField="0" baseItem="0"/>
-    <dataField name="环比" fld="3" baseField="0" baseItem="0"/>
-    <dataField name="新客户数" fld="5" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1177,7 +947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:O24"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -1206,13 +976,13 @@
       <c r="O1" s="8"/>
     </row>
     <row r="2" spans="2:15">
-      <c r="B2" s="15" t="str">
+      <c r="B2" s="10" t="str">
         <f>_input!$B2&amp;_input!$B3&amp;"趋势图"</f>
         <v>搜索+推广点击消费趋势图</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
       <c r="O2" s="8"/>
     </row>
     <row r="3" spans="2:15">
@@ -1297,120 +1067,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:D9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="11.75" customWidth="1"/>
-    <col min="3" max="3" width="7.75" customWidth="1"/>
-    <col min="4" max="4" width="9.75" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:4" ht="24" customHeight="1">
-      <c r="A2" s="16" t="str">
-        <f>_input2!$B2&amp;" "&amp;_input2!$B3&amp;"核心指标报表"</f>
-        <v>搜索+推广 日数据核心指标报表</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="11">
-        <v>1122</v>
-      </c>
-      <c r="C5" s="11">
-        <v>77</v>
-      </c>
-      <c r="D5" s="11">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="11">
-        <v>345</v>
-      </c>
-      <c r="C6" s="11">
-        <v>13</v>
-      </c>
-      <c r="D6" s="11">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="11">
-        <v>234</v>
-      </c>
-      <c r="C7" s="11">
-        <v>23</v>
-      </c>
-      <c r="D7" s="11">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="11">
-        <v>543</v>
-      </c>
-      <c r="C8" s="11">
-        <v>41</v>
-      </c>
-      <c r="D8" s="11">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="11">
-        <v>1122</v>
-      </c>
-      <c r="C9" s="11">
-        <v>77</v>
-      </c>
-      <c r="D9" s="11">
-        <v>676</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:D2"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FF7030A0"/>
@@ -1542,12 +1198,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1674,133 +1330,9 @@
         <v>3744123</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="13"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <tabColor rgb="FF7030A0"/>
-  </sheetPr>
-  <dimension ref="A1:F8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1">
-      <c r="A1" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="18" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6">
-        <v>345</v>
-      </c>
-      <c r="D6">
-        <v>13</v>
-      </c>
-      <c r="E6">
-        <v>7</v>
-      </c>
-      <c r="F6">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7">
-        <v>234</v>
-      </c>
-      <c r="D7">
-        <v>23</v>
-      </c>
-      <c r="E7">
-        <v>12</v>
-      </c>
-      <c r="F7">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8">
-        <v>543</v>
-      </c>
-      <c r="D8">
-        <v>41</v>
-      </c>
-      <c r="E8">
-        <v>23</v>
-      </c>
-      <c r="F8">
-        <v>321</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
rill-analysis: add column/row base support.
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/luopan.xlsx
+++ b/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/luopan.xlsx
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -244,6 +244,10 @@
   </si>
   <si>
     <t>json</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -255,7 +259,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,13 +274,6 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF222222"/>
-      <name val="Inherit"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -314,18 +311,12 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE5E5E5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -392,17 +383,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
@@ -410,23 +398,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -460,7 +445,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>_input!$A$5</c:f>
+              <c:f>_input!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -471,10 +456,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>_input!$B$4:$O$4</c:f>
+              <c:f>_input!$A$5:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>yyyy/m/d</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>40630</c:v>
                 </c:pt>
@@ -493,91 +478,43 @@
                 <c:pt idx="5">
                   <c:v>40635</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>40636</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>40637</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>40638</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>40639</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>40640</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40641</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>40642</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>40643</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>_input!$B$5:$O$5</c:f>
+              <c:f>_input!$B$5:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>3344110</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2344111</c:v>
+                  <c:v>3544111</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3344112</c:v>
+                  <c:v>3444111</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5344113</c:v>
+                  <c:v>3344111</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3344114</c:v>
+                  <c:v>3744111</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3344115</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3999116</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3344117</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3344118</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3544119</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3344120</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4244121</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2344122</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3744123</c:v>
+                  <c:v>4444111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64077184"/>
-        <c:axId val="80540032"/>
+        <c:axId val="65686144"/>
+        <c:axId val="80400768"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64077184"/>
+        <c:axId val="65686144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -586,13 +523,13 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80540032"/>
+        <c:crossAx val="80400768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="80540032"/>
+        <c:axId val="80400768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -601,7 +538,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64077184"/>
+        <c:crossAx val="65686144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -619,7 +556,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -973,88 +910,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15">
-      <c r="O1" s="8"/>
+      <c r="O1" s="7"/>
     </row>
     <row r="2" spans="2:15">
-      <c r="B2" s="10" t="str">
+      <c r="B2" s="8" t="str">
         <f>_input!$B2&amp;_input!$B3&amp;"趋势图"</f>
         <v>搜索+推广点击消费趋势图</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="O2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="O2" s="7"/>
     </row>
     <row r="3" spans="2:15">
-      <c r="O3" s="8"/>
+      <c r="O3" s="7"/>
     </row>
     <row r="4" spans="2:15">
-      <c r="B4" s="3" t="str">
+      <c r="B4" s="2" t="str">
         <f>_input!$B3</f>
         <v>点击消费</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="O4" s="8"/>
+      <c r="C4" s="2"/>
+      <c r="O4" s="7"/>
     </row>
     <row r="5" spans="2:15" ht="3" customHeight="1">
-      <c r="O5" s="8"/>
+      <c r="O5" s="7"/>
     </row>
     <row r="6" spans="2:15">
-      <c r="O6" s="8"/>
+      <c r="O6" s="7"/>
     </row>
     <row r="7" spans="2:15">
-      <c r="O7" s="8"/>
+      <c r="O7" s="7"/>
     </row>
     <row r="8" spans="2:15">
-      <c r="O8" s="8"/>
+      <c r="O8" s="7"/>
     </row>
     <row r="9" spans="2:15">
-      <c r="O9" s="8"/>
+      <c r="O9" s="7"/>
     </row>
     <row r="10" spans="2:15">
-      <c r="O10" s="8"/>
+      <c r="O10" s="7"/>
     </row>
     <row r="11" spans="2:15">
-      <c r="O11" s="8"/>
+      <c r="O11" s="7"/>
     </row>
     <row r="12" spans="2:15">
-      <c r="O12" s="8"/>
+      <c r="O12" s="7"/>
     </row>
     <row r="13" spans="2:15">
-      <c r="O13" s="8"/>
+      <c r="O13" s="7"/>
     </row>
     <row r="14" spans="2:15">
-      <c r="O14" s="8"/>
+      <c r="O14" s="7"/>
     </row>
     <row r="15" spans="2:15">
-      <c r="O15" s="8"/>
+      <c r="O15" s="7"/>
     </row>
     <row r="16" spans="2:15">
-      <c r="O16" s="8"/>
+      <c r="O16" s="7"/>
     </row>
     <row r="17" spans="15:15">
-      <c r="O17" s="8"/>
+      <c r="O17" s="7"/>
     </row>
     <row r="18" spans="15:15">
-      <c r="O18" s="8"/>
+      <c r="O18" s="7"/>
     </row>
     <row r="19" spans="15:15">
-      <c r="O19" s="8"/>
+      <c r="O19" s="7"/>
     </row>
     <row r="20" spans="15:15">
-      <c r="O20" s="8"/>
+      <c r="O20" s="7"/>
     </row>
     <row r="21" spans="15:15">
-      <c r="O21" s="8"/>
+      <c r="O21" s="7"/>
     </row>
     <row r="22" spans="15:15">
-      <c r="O22" s="8"/>
+      <c r="O22" s="7"/>
     </row>
     <row r="23" spans="15:15">
-      <c r="O23" s="8"/>
+      <c r="O23" s="7"/>
     </row>
     <row r="24" spans="15:15">
-      <c r="O24" s="8"/>
+      <c r="O24" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1088,102 +1025,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="2" t="str">
+      <c r="G3" s="1" t="str">
         <f>$D2</f>
         <v>用户</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="b">
+      <c r="B4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="2" t="str">
+      <c r="G4" s="1" t="str">
         <f>$D2</f>
         <v>用户</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="2" t="str">
+      <c r="G5" s="1" t="str">
         <f>$D2&amp;" "&amp;$D4</f>
         <v>用户 商业产品线</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1203,131 +1140,91 @@
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" customHeight="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" ht="18" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="18" customHeight="1">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:2" ht="18" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="18" customHeight="1" thickBot="1">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:2" ht="18" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="14.25" thickBot="1">
-      <c r="A4" s="1" t="str">
-        <f>$B2</f>
-        <v>搜索+推广</v>
-      </c>
-      <c r="B4" s="7">
+    <row r="4" spans="1:2" ht="14.25" thickBot="1">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25" thickBot="1">
+      <c r="A5" s="6">
         <v>40630</v>
       </c>
-      <c r="C4" s="7">
+      <c r="B5" s="3">
+        <v>3344110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14.25" thickBot="1">
+      <c r="A6" s="6">
         <v>40631</v>
       </c>
-      <c r="D4" s="7">
+      <c r="B6" s="3">
+        <v>3544111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.25" thickBot="1">
+      <c r="A7" s="6">
         <v>40632</v>
       </c>
-      <c r="E4" s="7">
+      <c r="B7" s="3">
+        <v>3444111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.25" thickBot="1">
+      <c r="A8" s="6">
         <v>40633</v>
       </c>
-      <c r="F4" s="7">
+      <c r="B8" s="3">
+        <v>3344111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.25" thickBot="1">
+      <c r="A9" s="6">
         <v>40634</v>
       </c>
-      <c r="G4" s="7">
+      <c r="B9" s="3">
+        <v>3744111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="14.25" thickBot="1">
+      <c r="A10" s="6">
         <v>40635</v>
       </c>
-      <c r="H4" s="7">
-        <v>40636</v>
-      </c>
-      <c r="I4" s="7">
-        <v>40637</v>
-      </c>
-      <c r="J4" s="7">
-        <v>40638</v>
-      </c>
-      <c r="K4" s="7">
-        <v>40639</v>
-      </c>
-      <c r="L4" s="7">
-        <v>40640</v>
-      </c>
-      <c r="M4" s="7">
-        <v>40641</v>
-      </c>
-      <c r="N4" s="7">
-        <v>40642</v>
-      </c>
-      <c r="O4" s="7">
-        <v>40643</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="14.25" thickBot="1">
-      <c r="A5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="4">
-        <v>3344110</v>
-      </c>
-      <c r="C5" s="4">
-        <v>2344111</v>
-      </c>
-      <c r="D5" s="4">
-        <v>3344112</v>
-      </c>
-      <c r="E5" s="4">
-        <v>5344113</v>
-      </c>
-      <c r="F5" s="4">
-        <v>3344114</v>
-      </c>
-      <c r="G5" s="4">
-        <v>3344115</v>
-      </c>
-      <c r="H5" s="4">
-        <v>3999116</v>
-      </c>
-      <c r="I5" s="4">
-        <v>3344117</v>
-      </c>
-      <c r="J5" s="4">
-        <v>3344118</v>
-      </c>
-      <c r="K5" s="4">
-        <v>3544119</v>
-      </c>
-      <c r="L5" s="4">
-        <v>3344120</v>
-      </c>
-      <c r="M5" s="4">
-        <v>4244121</v>
-      </c>
-      <c r="N5" s="4">
-        <v>2344122</v>
-      </c>
-      <c r="O5" s="4">
-        <v>3744123</v>
+      <c r="B10" s="3">
+        <v>4444111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rill-analysis: Enhance usability - base on luopan.xlsx
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/luopan.xlsx
+++ b/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/luopan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220"/>
@@ -144,12 +144,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Format</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -191,22 +215,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>line.action</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ind.action</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>管辖岗位</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>pos.action</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>select</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -252,6 +264,22 @@
   </si>
   <si>
     <t>高级经理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yyyy-MM-dd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost:8080/rill-analysis-report/web/example/pos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost:8080/rill-analysis-report/web/example/line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost:8080/rill-analysis-report/web/example/ind</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -388,7 +416,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -415,6 +443,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -510,11 +541,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="65686144"/>
-        <c:axId val="80400768"/>
+        <c:axId val="83539072"/>
+        <c:axId val="83540608"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="65686144"/>
+        <c:axId val="83539072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -523,13 +554,13 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80400768"/>
+        <c:crossAx val="83540608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="80400768"/>
+        <c:axId val="83540608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -538,7 +569,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65686144"/>
+        <c:crossAx val="83539072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -556,7 +587,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1008,7 +1039,7 @@
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1021,18 +1052,19 @@
     <col min="5" max="5" width="8.875" customWidth="1"/>
     <col min="6" max="6" width="19.375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.5" customWidth="1"/>
+    <col min="8" max="8" width="66" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1" t="s">
@@ -1040,8 +1072,11 @@
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1057,8 +1092,9 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1066,7 +1102,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5" t="s">
@@ -1076,11 +1112,12 @@
         <f>$D2</f>
         <v>用户</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="H3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1098,40 +1135,45 @@
         <f>$D2</f>
         <v>用户</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="H4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G5" s="1" t="str">
         <f>$D2&amp;" "&amp;$D4</f>
         <v>用户 商业产品线</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="H5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+    <hyperlink ref="H4" r:id="rId3"/>
+    <hyperlink ref="H5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1152,31 +1194,31 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" thickBot="1">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.25" thickBot="1">

</xml_diff>

<commit_message>
rill-analysis: Define json data retriever interface
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/luopan.xlsx
+++ b/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/luopan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="trend" sheetId="5" r:id="rId1"/>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -231,10 +231,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>data.action</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>点击消费</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -280,6 +276,30 @@
   </si>
   <si>
     <t>http://tc-crm-dp01.tc.baidu.com:8988/rill-analysis-report/web/example/ind</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2011/3/28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2011/3/29</t>
+  </si>
+  <si>
+    <t>2011/3/30</t>
+  </si>
+  <si>
+    <t>2011/4/01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2011/4/02</t>
+  </si>
+  <si>
+    <t>2011/4/03</t>
+  </si>
+  <si>
+    <t>http://tc-crm-dp01.tc.baidu.com:8988/rill-analysis-report/web/example/data</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -435,14 +455,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -486,31 +506,30 @@
             </c:strRef>
           </c:tx>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>_input!$A$5:$A$10</c:f>
-              <c:numCache>
-                <c:formatCode>yyyy/m/d</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40630</c:v>
+                  <c:v>2011/3/28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40631</c:v>
+                  <c:v>2011/3/29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40632</c:v>
+                  <c:v>2011/3/30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40633</c:v>
+                  <c:v>2011/4/01</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40634</c:v>
+                  <c:v>2011/4/02</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40635</c:v>
+                  <c:v>2011/4/03</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -541,11 +560,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="87266048"/>
-        <c:axId val="87267584"/>
+        <c:axId val="85758720"/>
+        <c:axId val="85760256"/>
       </c:lineChart>
-      <c:dateAx>
-        <c:axId val="87266048"/>
+      <c:catAx>
+        <c:axId val="85758720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -554,13 +573,14 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87267584"/>
+        <c:crossAx val="85760256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-      </c:dateAx>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="87267584"/>
+        <c:axId val="85760256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -569,7 +589,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87266048"/>
+        <c:crossAx val="85758720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -587,7 +607,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000411" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000411" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -915,7 +935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:O24"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -941,7 +961,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15">
-      <c r="O1" s="7"/>
+      <c r="O1" s="6"/>
     </row>
     <row r="2" spans="2:15">
       <c r="B2" s="9" t="str">
@@ -951,10 +971,10 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="O2" s="7"/>
+      <c r="O2" s="6"/>
     </row>
     <row r="3" spans="2:15">
-      <c r="O3" s="7"/>
+      <c r="O3" s="6"/>
     </row>
     <row r="4" spans="2:15">
       <c r="B4" s="2" t="str">
@@ -962,67 +982,67 @@
         <v>点击消费</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="O4" s="7"/>
+      <c r="O4" s="6"/>
     </row>
     <row r="5" spans="2:15" ht="3" customHeight="1">
-      <c r="O5" s="7"/>
+      <c r="O5" s="6"/>
     </row>
     <row r="6" spans="2:15">
-      <c r="O6" s="7"/>
+      <c r="O6" s="6"/>
     </row>
     <row r="7" spans="2:15">
-      <c r="O7" s="7"/>
+      <c r="O7" s="6"/>
     </row>
     <row r="8" spans="2:15">
-      <c r="O8" s="7"/>
+      <c r="O8" s="6"/>
     </row>
     <row r="9" spans="2:15">
-      <c r="O9" s="7"/>
+      <c r="O9" s="6"/>
     </row>
     <row r="10" spans="2:15">
-      <c r="O10" s="7"/>
+      <c r="O10" s="6"/>
     </row>
     <row r="11" spans="2:15">
-      <c r="O11" s="7"/>
+      <c r="O11" s="6"/>
     </row>
     <row r="12" spans="2:15">
-      <c r="O12" s="7"/>
+      <c r="O12" s="6"/>
     </row>
     <row r="13" spans="2:15">
-      <c r="O13" s="7"/>
+      <c r="O13" s="6"/>
     </row>
     <row r="14" spans="2:15">
-      <c r="O14" s="7"/>
+      <c r="O14" s="6"/>
     </row>
     <row r="15" spans="2:15">
-      <c r="O15" s="7"/>
+      <c r="O15" s="6"/>
     </row>
     <row r="16" spans="2:15">
-      <c r="O16" s="7"/>
+      <c r="O16" s="6"/>
     </row>
     <row r="17" spans="15:15">
-      <c r="O17" s="7"/>
+      <c r="O17" s="6"/>
     </row>
     <row r="18" spans="15:15">
-      <c r="O18" s="7"/>
+      <c r="O18" s="6"/>
     </row>
     <row r="19" spans="15:15">
-      <c r="O19" s="7"/>
+      <c r="O19" s="6"/>
     </row>
     <row r="20" spans="15:15">
-      <c r="O20" s="7"/>
+      <c r="O20" s="6"/>
     </row>
     <row r="21" spans="15:15">
-      <c r="O21" s="7"/>
+      <c r="O21" s="6"/>
     </row>
     <row r="22" spans="15:15">
-      <c r="O22" s="7"/>
+      <c r="O22" s="6"/>
     </row>
     <row r="23" spans="15:15">
-      <c r="O23" s="7"/>
+      <c r="O23" s="6"/>
     </row>
     <row r="24" spans="15:15">
-      <c r="O24" s="7"/>
+      <c r="O24" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1041,7 +1061,9 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -1073,7 +1095,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1112,8 +1134,8 @@
         <f>$D2</f>
         <v>用户</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>24</v>
+      <c r="H3" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="I3" s="1"/>
     </row>
@@ -1135,17 +1157,17 @@
         <f>$D2</f>
         <v>用户</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>25</v>
+      <c r="H4" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
@@ -1158,8 +1180,8 @@
         <f>$D2&amp;" "&amp;$D4</f>
         <v>用户 商业产品线</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>26</v>
+      <c r="H5" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="I5" s="1"/>
     </row>
@@ -1193,77 +1215,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>14</v>
+      <c r="A1" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" thickBot="1">
       <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="5" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A5" s="6">
-        <v>40630</v>
+      <c r="A5" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="B5" s="3">
         <v>3344110</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A6" s="6">
-        <v>40631</v>
+      <c r="A6" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="B6" s="3">
         <v>3544111</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A7" s="6">
-        <v>40632</v>
+      <c r="A7" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="B7" s="3">
         <v>3444111</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A8" s="6">
-        <v>40633</v>
+      <c r="A8" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B8" s="3">
         <v>3344111</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A9" s="6">
-        <v>40634</v>
+      <c r="A9" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="B9" s="3">
         <v>3744111</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A10" s="6">
-        <v>40635</v>
+      <c r="A10" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="B10" s="3">
         <v>4444111</v>
@@ -1271,7 +1293,10 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rill-analysis: Refactor report parameter configuration
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/luopan.xlsx
+++ b/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/luopan.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="trend" sheetId="5" r:id="rId1"/>
@@ -48,132 +48,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>作者:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Parameters</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>作者:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Type</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>作者:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Dependencies</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>作者:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fetch URL</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>作者:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Format</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -195,10 +75,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>用户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>provided</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -211,35 +87,123 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>管辖岗位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击消费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商业产品线</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>搜索+推广</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>分析指标</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>管辖岗位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>dataType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>json</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高级经理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yyyy-MM-dd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2011/3/28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2011/3/29</t>
+  </si>
+  <si>
+    <t>2011/3/30</t>
+  </si>
+  <si>
+    <t>2011/4/01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2011/4/02</t>
+  </si>
+  <si>
+    <t>2011/4/03</t>
   </si>
   <si>
     <t>选择日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>http://localhost:7070/rill-analysis-web/web/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>点击消费</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>商业产品线</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>搜索+推广</t>
+    <t>日期类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>posIds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lineId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>indId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>依赖关系</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>格式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>参数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dateType</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -247,59 +211,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>dataType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>json</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>高级经理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>yyyy-MM-dd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://tc-crm-dp01.tc.baidu.com:8988/rill-analysis-report/web/example/pos</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://tc-crm-dp01.tc.baidu.com:8988/rill-analysis-report/web/example/line</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://tc-crm-dp01.tc.baidu.com:8988/rill-analysis-report/web/example/ind</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2011/3/28</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2011/3/29</t>
-  </si>
-  <si>
-    <t>2011/3/30</t>
-  </si>
-  <si>
-    <t>2011/4/01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2011/4/02</t>
-  </si>
-  <si>
-    <t>2011/4/03</t>
-  </si>
-  <si>
-    <t>http://tc-crm-dp01.tc.baidu.com:8988/rill-analysis-report/web/example/data</t>
+    <t>example/pos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>example/line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>example/ind</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>example/data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost:8080/rill-analysis-report/web/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -359,7 +287,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -378,8 +306,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor theme="6" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -426,6 +360,113 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -436,7 +477,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -449,20 +490,62 @@
     <xf numFmtId="3" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -472,7 +555,173 @@
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -560,11 +809,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="85758720"/>
-        <c:axId val="85760256"/>
+        <c:axId val="57952896"/>
+        <c:axId val="71426432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85758720"/>
+        <c:axId val="57952896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -573,14 +822,14 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85760256"/>
+        <c:crossAx val="71426432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85760256"/>
+        <c:axId val="71426432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -589,14 +838,13 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85758720"/>
+        <c:crossAx val="57952896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -607,7 +855,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000411" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000411" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000544" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000544" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -646,6 +894,24 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="paramTable" displayName="paramTable" ref="A8:G13" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="A8:G13"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="参数" dataDxfId="6"/>
+    <tableColumn id="2" name="名称" dataDxfId="5"/>
+    <tableColumn id="3" name="值" dataDxfId="4"/>
+    <tableColumn id="4" name="类型" dataDxfId="3"/>
+    <tableColumn id="5" name="依赖关系" dataDxfId="2">
+      <calculatedColumnFormula>$B8</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="源" dataDxfId="1" dataCellStyle="超链接"/>
+    <tableColumn id="7" name="格式" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -935,7 +1201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:O24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -961,20 +1227,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15">
-      <c r="O1" s="6"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="2:15">
-      <c r="B2" s="9" t="str">
+      <c r="B2" s="23" t="str">
         <f>_input!$B2&amp;_input!$B3&amp;"趋势图"</f>
         <v>搜索+推广点击消费趋势图</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="O2" s="6"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="O2" s="5"/>
     </row>
     <row r="3" spans="2:15">
-      <c r="O3" s="6"/>
+      <c r="O3" s="5"/>
     </row>
     <row r="4" spans="2:15">
       <c r="B4" s="2" t="str">
@@ -982,67 +1248,67 @@
         <v>点击消费</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="O4" s="6"/>
+      <c r="O4" s="5"/>
     </row>
     <row r="5" spans="2:15" ht="3" customHeight="1">
-      <c r="O5" s="6"/>
+      <c r="O5" s="5"/>
     </row>
     <row r="6" spans="2:15">
-      <c r="O6" s="6"/>
+      <c r="O6" s="5"/>
     </row>
     <row r="7" spans="2:15">
-      <c r="O7" s="6"/>
+      <c r="O7" s="5"/>
     </row>
     <row r="8" spans="2:15">
-      <c r="O8" s="6"/>
+      <c r="O8" s="5"/>
     </row>
     <row r="9" spans="2:15">
-      <c r="O9" s="6"/>
+      <c r="O9" s="5"/>
     </row>
     <row r="10" spans="2:15">
-      <c r="O10" s="6"/>
+      <c r="O10" s="5"/>
     </row>
     <row r="11" spans="2:15">
-      <c r="O11" s="6"/>
+      <c r="O11" s="5"/>
     </row>
     <row r="12" spans="2:15">
-      <c r="O12" s="6"/>
+      <c r="O12" s="5"/>
     </row>
     <row r="13" spans="2:15">
-      <c r="O13" s="6"/>
+      <c r="O13" s="5"/>
     </row>
     <row r="14" spans="2:15">
-      <c r="O14" s="6"/>
+      <c r="O14" s="5"/>
     </row>
     <row r="15" spans="2:15">
-      <c r="O15" s="6"/>
+      <c r="O15" s="5"/>
     </row>
     <row r="16" spans="2:15">
-      <c r="O16" s="6"/>
+      <c r="O16" s="5"/>
     </row>
     <row r="17" spans="15:15">
-      <c r="O17" s="6"/>
+      <c r="O17" s="5"/>
     </row>
     <row r="18" spans="15:15">
-      <c r="O18" s="6"/>
+      <c r="O18" s="5"/>
     </row>
     <row r="19" spans="15:15">
-      <c r="O19" s="6"/>
+      <c r="O19" s="5"/>
     </row>
     <row r="20" spans="15:15">
-      <c r="O20" s="6"/>
+      <c r="O20" s="5"/>
     </row>
     <row r="21" spans="15:15">
-      <c r="O21" s="6"/>
+      <c r="O21" s="5"/>
     </row>
     <row r="22" spans="15:15">
-      <c r="O22" s="6"/>
+      <c r="O22" s="5"/>
     </row>
     <row r="23" spans="15:15">
-      <c r="O23" s="6"/>
+      <c r="O23" s="5"/>
     </row>
     <row r="24" spans="15:15">
-      <c r="O24" s="6"/>
+      <c r="O24" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1059,143 +1325,181 @@
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.125" customWidth="1"/>
-    <col min="3" max="3" width="1.25" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.875" customWidth="1"/>
-    <col min="6" max="6" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="82.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.75" customWidth="1"/>
+    <col min="3" max="3" width="6.875" customWidth="1"/>
+    <col min="4" max="4" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.875" customWidth="1"/>
+    <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:7" ht="54" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="B1" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="17"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="18"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="1" t="str">
-        <f>$D2</f>
-        <v>用户</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="1" t="str">
-        <f>$D2</f>
-        <v>用户</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="1" t="str">
-        <f>$D2&amp;" "&amp;$D4</f>
-        <v>用户 商业产品线</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="1"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="17" t="str">
+        <f t="shared" ref="E13" si="0">$B12</f>
+        <v>lineId</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2"/>
-    <hyperlink ref="H4" r:id="rId3"/>
-    <hyperlink ref="H5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId5"/>
-  <legacyDrawing r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1215,77 +1519,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" customHeight="1">
-      <c r="A1" s="4" t="s">
-        <v>32</v>
+      <c r="A1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" thickBot="1">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A5" s="8" t="s">
-        <v>26</v>
+      <c r="A5" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="B5" s="3">
         <v>3344110</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A6" s="8" t="s">
-        <v>27</v>
+      <c r="A6" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="B6" s="3">
         <v>3544111</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A7" s="8" t="s">
-        <v>28</v>
+      <c r="A7" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B7" s="3">
         <v>3444111</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A8" s="8" t="s">
-        <v>29</v>
+      <c r="A8" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="B8" s="3">
         <v>3344111</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A9" s="8" t="s">
-        <v>30</v>
+      <c r="A9" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="B9" s="3">
         <v>3744111</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A10" s="8" t="s">
-        <v>31</v>
+      <c r="A10" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="B10" s="3">
         <v>4444111</v>
@@ -1293,10 +1597,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rill-analysis: Add chart x-series smart show.
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/luopan.xlsx
+++ b/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/luopan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220" activeTab="1"/>
@@ -235,7 +235,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,14 +256,6 @@
       <color rgb="FF222222"/>
       <name val="Inherit"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
@@ -313,7 +305,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -456,28 +448,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="6"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -496,7 +473,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
@@ -541,9 +518,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -551,9 +525,8 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -809,11 +782,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="57952896"/>
-        <c:axId val="71426432"/>
+        <c:axId val="94253440"/>
+        <c:axId val="94254976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57952896"/>
+        <c:axId val="94253440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -822,14 +795,14 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71426432"/>
+        <c:crossAx val="94254976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71426432"/>
+        <c:axId val="94254976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -838,7 +811,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57952896"/>
+        <c:crossAx val="94253440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -855,7 +828,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000544" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000544" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000588" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000588" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -907,7 +880,7 @@
     <tableColumn id="5" name="依赖关系" dataDxfId="2">
       <calculatedColumnFormula>$B8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="源" dataDxfId="1" dataCellStyle="超链接"/>
+    <tableColumn id="6" name="源" dataDxfId="1"/>
     <tableColumn id="7" name="格式" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1230,13 +1203,13 @@
       <c r="O1" s="5"/>
     </row>
     <row r="2" spans="2:15">
-      <c r="B2" s="23" t="str">
+      <c r="B2" s="22" t="str">
         <f>_input!$B2&amp;_input!$B3&amp;"趋势图"</f>
         <v>搜索+推广点击消费趋势图</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
       <c r="O2" s="5"/>
     </row>
     <row r="3" spans="2:15">
@@ -1344,12 +1317,12 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -1491,14 +1464,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>